<commit_message>
add docstrings and checks for bugs and null pointers
</commit_message>
<xml_diff>
--- a/results/language_distribution/bilingual_percentage.xlsx
+++ b/results/language_distribution/bilingual_percentage.xlsx
@@ -444,16 +444,16 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E2">
-        <v>34.92063492063492</v>
+        <v>34.21052631578947</v>
       </c>
       <c r="F2">
-        <v>65.07936507936508</v>
+        <v>65.78947368421053</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -464,16 +464,16 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D3">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3">
-        <v>62.17391304347826</v>
+        <v>62.39316239316239</v>
       </c>
       <c r="F3">
-        <v>37.82608695652173</v>
+        <v>37.60683760683761</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -487,13 +487,13 @@
         <v>117</v>
       </c>
       <c r="D4">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4">
-        <v>46.24505928853755</v>
+        <v>46.42857142857143</v>
       </c>
       <c r="F4">
-        <v>53.75494071146245</v>
+        <v>53.57142857142857</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -507,13 +507,13 @@
         <v>80</v>
       </c>
       <c r="D5">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5">
-        <v>52.98013245033113</v>
+        <v>53.33333333333334</v>
       </c>
       <c r="F5">
-        <v>47.01986754966887</v>
+        <v>46.66666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -541,10 +541,10 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>47.62931034482759</v>
+        <v>47.6906552094522</v>
       </c>
       <c r="F7">
-        <v>52.37068965517241</v>
+        <v>52.3093447905478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initialize conda virualenv and modifications on topic_analysis
</commit_message>
<xml_diff>
--- a/results/language_distribution/bilingual_percentage.xlsx
+++ b/results/language_distribution/bilingual_percentage.xlsx
@@ -444,16 +444,16 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E2">
-        <v>34.21052631578947</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="F2">
-        <v>65.78947368421053</v>
+        <v>66.66666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -464,16 +464,16 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D3">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3">
-        <v>62.39316239316239</v>
+        <v>62.82051282051282</v>
       </c>
       <c r="F3">
-        <v>37.60683760683761</v>
+        <v>37.17948717948718</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -484,16 +484,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4">
         <v>135</v>
       </c>
       <c r="E4">
-        <v>46.42857142857143</v>
+        <v>46.21513944223107</v>
       </c>
       <c r="F4">
-        <v>53.57142857142857</v>
+        <v>53.78486055776892</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -541,10 +541,10 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>47.6906552094522</v>
+        <v>47.57804090419806</v>
       </c>
       <c r="F7">
-        <v>52.3093447905478</v>
+        <v>52.42195909580194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regular testing and minor changes
</commit_message>
<xml_diff>
--- a/results/language_distribution/bilingual_percentage.xlsx
+++ b/results/language_distribution/bilingual_percentage.xlsx
@@ -444,16 +444,16 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E2">
-        <v>33.33333333333333</v>
+        <v>34.39153439153439</v>
       </c>
       <c r="F2">
-        <v>66.66666666666666</v>
+        <v>65.60846560846561</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -464,16 +464,16 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D3">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3">
-        <v>62.82051282051282</v>
+        <v>63.24786324786324</v>
       </c>
       <c r="F3">
-        <v>37.17948717948718</v>
+        <v>36.75213675213676</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -504,16 +504,16 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5">
-        <v>53.33333333333334</v>
+        <v>52.66666666666666</v>
       </c>
       <c r="F5">
-        <v>46.66666666666666</v>
+        <v>47.33333333333334</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -541,10 +541,10 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>47.57804090419806</v>
+        <v>47.79332615715823</v>
       </c>
       <c r="F7">
-        <v>52.42195909580194</v>
+        <v>52.20667384284177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>